<commit_message>
Add new generated output files
</commit_message>
<xml_diff>
--- a/udemy-scraper/out_files/udemy_courses.xlsx
+++ b/udemy-scraper/out_files/udemy_courses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -826,8 +826,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -881,22 +881,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -934,7 +929,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -968,7 +963,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1003,10 +997,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1179,23 +1172,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="101" width="20.6640625" customWidth="1"/>
+    <col min="2" max="101" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1214,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2">
         <v>24</v>
       </c>
@@ -1244,13 +1231,13 @@
         <v>13</v>
       </c>
       <c r="F2" s="2">
-        <v>153501</v>
+        <v>153524</v>
       </c>
       <c r="G2" s="2">
-        <v>6235</v>
+        <v>6241</v>
       </c>
       <c r="H2" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
@@ -1259,7 +1246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1276,10 +1263,10 @@
         <v>13</v>
       </c>
       <c r="F3" s="2">
-        <v>150297</v>
+        <v>150364</v>
       </c>
       <c r="G3" s="2">
-        <v>31705</v>
+        <v>31715</v>
       </c>
       <c r="H3" s="2">
         <v>4.5</v>
@@ -1291,7 +1278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
         <v>10</v>
       </c>
@@ -1308,10 +1295,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="2">
-        <v>96466</v>
+        <v>96548</v>
       </c>
       <c r="G4" s="2">
-        <v>19244</v>
+        <v>19262</v>
       </c>
       <c r="H4" s="2">
         <v>4.7</v>
@@ -1323,7 +1310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1340,13 +1327,13 @@
         <v>13</v>
       </c>
       <c r="F5" s="2">
-        <v>58818</v>
+        <v>58850</v>
       </c>
       <c r="G5" s="2">
         <v>13257</v>
       </c>
       <c r="H5" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>29</v>
@@ -1355,7 +1342,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1372,10 +1359,10 @@
         <v>13</v>
       </c>
       <c r="F6" s="2">
-        <v>47513</v>
+        <v>47517</v>
       </c>
       <c r="G6" s="2">
-        <v>2328</v>
+        <v>2329</v>
       </c>
       <c r="H6" s="2">
         <v>4.5</v>
@@ -1387,7 +1374,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="2">
         <v>11</v>
       </c>
@@ -1404,10 +1391,10 @@
         <v>13</v>
       </c>
       <c r="F7" s="2">
-        <v>39140</v>
+        <v>39166</v>
       </c>
       <c r="G7" s="2">
-        <v>6510</v>
+        <v>6514</v>
       </c>
       <c r="H7" s="2">
         <v>4.7</v>
@@ -1419,7 +1406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="2">
         <v>26</v>
       </c>
@@ -1436,10 +1423,10 @@
         <v>13</v>
       </c>
       <c r="F8" s="2">
-        <v>39140</v>
+        <v>39166</v>
       </c>
       <c r="G8" s="2">
-        <v>6510</v>
+        <v>6514</v>
       </c>
       <c r="H8" s="2">
         <v>4.7</v>
@@ -1451,7 +1438,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="2">
         <v>45</v>
       </c>
@@ -1468,13 +1455,13 @@
         <v>13</v>
       </c>
       <c r="F9" s="2">
-        <v>38747</v>
+        <v>38760</v>
       </c>
       <c r="G9" s="2">
-        <v>6440</v>
+        <v>6458</v>
       </c>
       <c r="H9" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>43</v>
@@ -1483,7 +1470,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10" s="2">
         <v>27</v>
       </c>
@@ -1506,7 +1493,7 @@
         <v>462</v>
       </c>
       <c r="H10" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>48</v>
@@ -1515,7 +1502,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" s="2">
         <v>44</v>
       </c>
@@ -1532,13 +1519,13 @@
         <v>13</v>
       </c>
       <c r="F11" s="2">
-        <v>32628</v>
+        <v>32697</v>
       </c>
       <c r="G11" s="2">
-        <v>6951</v>
+        <v>6955</v>
       </c>
       <c r="H11" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>53</v>
@@ -1547,7 +1534,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -1564,10 +1551,10 @@
         <v>13</v>
       </c>
       <c r="F12" s="2">
-        <v>31453</v>
+        <v>31466</v>
       </c>
       <c r="G12" s="2">
-        <v>5681</v>
+        <v>5695</v>
       </c>
       <c r="H12" s="2">
         <v>4.5</v>
@@ -1579,7 +1566,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13" s="2">
         <v>33</v>
       </c>
@@ -1596,13 +1583,13 @@
         <v>13</v>
       </c>
       <c r="F13" s="2">
-        <v>27305</v>
+        <v>27316</v>
       </c>
       <c r="G13" s="2">
         <v>3869</v>
       </c>
       <c r="H13" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>62</v>
@@ -1611,7 +1598,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14" s="2">
         <v>15</v>
       </c>
@@ -1628,10 +1615,10 @@
         <v>13</v>
       </c>
       <c r="F14" s="2">
-        <v>27077</v>
+        <v>27088</v>
       </c>
       <c r="G14" s="2">
-        <v>4560</v>
+        <v>4561</v>
       </c>
       <c r="H14" s="2">
         <v>4.7</v>
@@ -1643,7 +1630,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15" s="2">
         <v>32</v>
       </c>
@@ -1660,10 +1647,10 @@
         <v>13</v>
       </c>
       <c r="F15" s="2">
-        <v>25981</v>
+        <v>26009</v>
       </c>
       <c r="G15" s="2">
-        <v>5683</v>
+        <v>5688</v>
       </c>
       <c r="H15" s="2">
         <v>4.5</v>
@@ -1675,7 +1662,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" s="2">
         <v>8</v>
       </c>
@@ -1692,10 +1679,10 @@
         <v>13</v>
       </c>
       <c r="F16" s="2">
-        <v>23830</v>
+        <v>23935</v>
       </c>
       <c r="G16" s="2">
-        <v>3807</v>
+        <v>3835</v>
       </c>
       <c r="H16" s="2">
         <v>4.8</v>
@@ -1707,7 +1694,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -1724,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="2">
-        <v>21263</v>
+        <v>21301</v>
       </c>
       <c r="G17" s="2">
         <v>1077</v>
@@ -1739,7 +1726,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="2">
         <v>36</v>
       </c>
@@ -1756,13 +1743,13 @@
         <v>13</v>
       </c>
       <c r="F18" s="2">
-        <v>20601</v>
+        <v>20636</v>
       </c>
       <c r="G18" s="2">
-        <v>5284</v>
+        <v>5291</v>
       </c>
       <c r="H18" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>86</v>
@@ -1771,7 +1758,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19" s="2">
         <v>9</v>
       </c>
@@ -1788,13 +1775,13 @@
         <v>13</v>
       </c>
       <c r="F19" s="2">
-        <v>19299</v>
+        <v>19311</v>
       </c>
       <c r="G19" s="2">
-        <v>3982</v>
+        <v>3985</v>
       </c>
       <c r="H19" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>91</v>
@@ -1803,7 +1790,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" s="2">
         <v>46</v>
       </c>
@@ -1820,7 +1807,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="2">
-        <v>18477</v>
+        <v>18490</v>
       </c>
       <c r="G20" s="2">
         <v>2631</v>
@@ -1835,7 +1822,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -1852,10 +1839,10 @@
         <v>13</v>
       </c>
       <c r="F21" s="2">
-        <v>18002</v>
+        <v>18007</v>
       </c>
       <c r="G21" s="2">
-        <v>4456</v>
+        <v>4458</v>
       </c>
       <c r="H21" s="2">
         <v>4.7</v>
@@ -1867,7 +1854,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" s="2">
         <v>14</v>
       </c>
@@ -1884,13 +1871,13 @@
         <v>13</v>
       </c>
       <c r="F22" s="2">
-        <v>16228</v>
+        <v>16241</v>
       </c>
       <c r="G22" s="2">
-        <v>1992</v>
+        <v>1995</v>
       </c>
       <c r="H22" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>104</v>
@@ -1899,7 +1886,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="2">
         <v>30</v>
       </c>
@@ -1916,10 +1903,10 @@
         <v>13</v>
       </c>
       <c r="F23" s="2">
-        <v>14716</v>
+        <v>14736</v>
       </c>
       <c r="G23" s="2">
-        <v>4757</v>
+        <v>4766</v>
       </c>
       <c r="H23" s="2">
         <v>4.7</v>
@@ -1931,7 +1918,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>25</v>
       </c>
@@ -1948,13 +1935,13 @@
         <v>13</v>
       </c>
       <c r="F24" s="2">
-        <v>14391</v>
+        <v>14399</v>
       </c>
       <c r="G24" s="2">
-        <v>3273</v>
+        <v>3277</v>
       </c>
       <c r="H24" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>113</v>
@@ -1963,7 +1950,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25" s="2">
         <v>29</v>
       </c>
@@ -1980,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="F25" s="2">
-        <v>13989</v>
+        <v>13999</v>
       </c>
       <c r="G25" s="2">
         <v>1853</v>
@@ -1995,7 +1982,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <v>20</v>
       </c>
@@ -2012,13 +1999,13 @@
         <v>13</v>
       </c>
       <c r="F26" s="2">
-        <v>13295</v>
+        <v>13303</v>
       </c>
       <c r="G26" s="2">
-        <v>2182</v>
+        <v>2183</v>
       </c>
       <c r="H26" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>121</v>
@@ -2027,7 +2014,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>43</v>
       </c>
@@ -2044,10 +2031,10 @@
         <v>13</v>
       </c>
       <c r="F27" s="2">
-        <v>12909</v>
+        <v>12916</v>
       </c>
       <c r="G27" s="2">
-        <v>4995</v>
+        <v>4996</v>
       </c>
       <c r="H27" s="2">
         <v>4.5</v>
@@ -2059,7 +2046,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" s="2">
         <v>48</v>
       </c>
@@ -2082,7 +2069,7 @@
         <v>116</v>
       </c>
       <c r="H28" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>131</v>
@@ -2091,7 +2078,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29" s="2">
         <v>47</v>
       </c>
@@ -2123,7 +2110,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30" s="2">
         <v>31</v>
       </c>
@@ -2140,13 +2127,13 @@
         <v>13</v>
       </c>
       <c r="F30" s="2">
-        <v>9926</v>
+        <v>9928</v>
       </c>
       <c r="G30" s="2">
-        <v>3444</v>
+        <v>3447</v>
       </c>
       <c r="H30" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>141</v>
@@ -2155,7 +2142,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" s="2">
         <v>34</v>
       </c>
@@ -2187,7 +2174,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32" s="2">
         <v>23</v>
       </c>
@@ -2204,13 +2191,13 @@
         <v>13</v>
       </c>
       <c r="F32" s="2">
-        <v>8693</v>
+        <v>8699</v>
       </c>
       <c r="G32" s="2">
-        <v>2072</v>
+        <v>2080</v>
       </c>
       <c r="H32" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>151</v>
@@ -2219,7 +2206,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" s="2">
         <v>5</v>
       </c>
@@ -2236,13 +2223,13 @@
         <v>13</v>
       </c>
       <c r="F33" s="2">
-        <v>8249</v>
+        <v>8253</v>
       </c>
       <c r="G33" s="2">
-        <v>1948</v>
+        <v>1952</v>
       </c>
       <c r="H33" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>156</v>
@@ -2251,7 +2238,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" s="2">
         <v>28</v>
       </c>
@@ -2268,13 +2255,13 @@
         <v>13</v>
       </c>
       <c r="F34" s="2">
-        <v>5550</v>
+        <v>5551</v>
       </c>
       <c r="G34" s="2">
         <v>1354</v>
       </c>
       <c r="H34" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>161</v>
@@ -2283,7 +2270,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35" s="2">
         <v>12</v>
       </c>
@@ -2300,7 +2287,7 @@
         <v>13</v>
       </c>
       <c r="F35" s="2">
-        <v>5154</v>
+        <v>5157</v>
       </c>
       <c r="G35" s="2">
         <v>694</v>
@@ -2315,7 +2302,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" s="2">
         <v>40</v>
       </c>
@@ -2338,7 +2325,7 @@
         <v>108</v>
       </c>
       <c r="H36" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>170</v>
@@ -2347,7 +2334,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" s="2">
         <v>38</v>
       </c>
@@ -2379,7 +2366,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" s="2">
         <v>21</v>
       </c>
@@ -2402,7 +2389,7 @@
         <v>327</v>
       </c>
       <c r="H38" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>179</v>
@@ -2411,7 +2398,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39" s="2">
         <v>22</v>
       </c>
@@ -2428,13 +2415,13 @@
         <v>13</v>
       </c>
       <c r="F39" s="2">
-        <v>3018</v>
+        <v>3019</v>
       </c>
       <c r="G39" s="2">
         <v>537</v>
       </c>
       <c r="H39" s="2">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>184</v>
@@ -2443,7 +2430,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40" s="2">
         <v>49</v>
       </c>
@@ -2460,13 +2447,13 @@
         <v>13</v>
       </c>
       <c r="F40" s="2">
-        <v>2983</v>
+        <v>2984</v>
       </c>
       <c r="G40" s="2">
         <v>456</v>
       </c>
       <c r="H40" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>189</v>
@@ -2475,7 +2462,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41" s="2">
         <v>19</v>
       </c>
@@ -2495,7 +2482,7 @@
         <v>2910</v>
       </c>
       <c r="G41" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H41" s="2">
         <v>4.7</v>
@@ -2507,7 +2494,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2539,7 +2526,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -2556,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="F43" s="2">
-        <v>2796</v>
+        <v>2798</v>
       </c>
       <c r="G43" s="2">
         <v>80</v>
@@ -2571,7 +2558,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44" s="2">
         <v>16</v>
       </c>
@@ -2588,7 +2575,7 @@
         <v>13</v>
       </c>
       <c r="F44" s="2">
-        <v>2633</v>
+        <v>2639</v>
       </c>
       <c r="G44" s="2">
         <v>483</v>
@@ -2603,7 +2590,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -2626,7 +2613,7 @@
         <v>381</v>
       </c>
       <c r="H45" s="2">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>212</v>
@@ -2635,7 +2622,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" s="2">
         <v>42</v>
       </c>
@@ -2652,13 +2639,13 @@
         <v>13</v>
       </c>
       <c r="F46" s="2">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="G46" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H46" s="2">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>216</v>
@@ -2667,7 +2654,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47" s="2">
         <v>35</v>
       </c>
@@ -2699,7 +2686,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10">
       <c r="A48" s="2">
         <v>18</v>
       </c>
@@ -2731,7 +2718,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10">
       <c r="A49" s="2">
         <v>37</v>
       </c>
@@ -2763,7 +2750,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2786,7 +2773,7 @@
         <v>26</v>
       </c>
       <c r="H50" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>234</v>

</xml_diff>

<commit_message>
remove unused http headers
</commit_message>
<xml_diff>
--- a/udemy-scraper/out_files/udemy_courses.xlsx
+++ b/udemy-scraper/out_files/udemy_courses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -826,8 +826,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -881,17 +881,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -929,7 +934,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -963,6 +968,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -997,9 +1003,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1172,17 +1179,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="101" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="101" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>24</v>
       </c>
@@ -1237,7 +1253,7 @@
         <v>6241</v>
       </c>
       <c r="H2" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
@@ -1246,7 +1262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1278,7 +1294,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>10</v>
       </c>
@@ -1310,7 +1326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1333,7 +1349,7 @@
         <v>13257</v>
       </c>
       <c r="H5" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>29</v>
@@ -1342,7 +1358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1374,7 +1390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>11</v>
       </c>
@@ -1406,7 +1422,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>26</v>
       </c>
@@ -1438,7 +1454,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45</v>
       </c>
@@ -1461,7 +1477,7 @@
         <v>6458</v>
       </c>
       <c r="H9" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>43</v>
@@ -1470,7 +1486,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>27</v>
       </c>
@@ -1493,7 +1509,7 @@
         <v>462</v>
       </c>
       <c r="H10" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>48</v>
@@ -1502,7 +1518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44</v>
       </c>
@@ -1525,7 +1541,7 @@
         <v>6955</v>
       </c>
       <c r="H11" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>53</v>
@@ -1534,7 +1550,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -1566,7 +1582,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>33</v>
       </c>
@@ -1589,7 +1605,7 @@
         <v>3869</v>
       </c>
       <c r="H13" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>62</v>
@@ -1598,7 +1614,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>15</v>
       </c>
@@ -1630,7 +1646,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>32</v>
       </c>
@@ -1662,7 +1678,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>8</v>
       </c>
@@ -1694,7 +1710,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -1726,7 +1742,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>36</v>
       </c>
@@ -1758,7 +1774,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>9</v>
       </c>
@@ -1781,7 +1797,7 @@
         <v>3985</v>
       </c>
       <c r="H19" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>91</v>
@@ -1790,7 +1806,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>46</v>
       </c>
@@ -1822,7 +1838,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -1854,7 +1870,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>14</v>
       </c>
@@ -1877,7 +1893,7 @@
         <v>1995</v>
       </c>
       <c r="H22" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>104</v>
@@ -1886,7 +1902,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>30</v>
       </c>
@@ -1918,7 +1934,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>25</v>
       </c>
@@ -1941,7 +1957,7 @@
         <v>3277</v>
       </c>
       <c r="H24" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>113</v>
@@ -1950,7 +1966,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>29</v>
       </c>
@@ -1982,7 +1998,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>20</v>
       </c>
@@ -2005,7 +2021,7 @@
         <v>2183</v>
       </c>
       <c r="H26" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>121</v>
@@ -2014,7 +2030,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43</v>
       </c>
@@ -2046,7 +2062,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>48</v>
       </c>
@@ -2069,7 +2085,7 @@
         <v>116</v>
       </c>
       <c r="H28" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>131</v>
@@ -2078,7 +2094,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>47</v>
       </c>
@@ -2110,7 +2126,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>31</v>
       </c>
@@ -2133,7 +2149,7 @@
         <v>3447</v>
       </c>
       <c r="H30" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>141</v>
@@ -2142,7 +2158,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>34</v>
       </c>
@@ -2174,7 +2190,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>23</v>
       </c>
@@ -2197,7 +2213,7 @@
         <v>2080</v>
       </c>
       <c r="H32" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>151</v>
@@ -2206,7 +2222,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>5</v>
       </c>
@@ -2229,7 +2245,7 @@
         <v>1952</v>
       </c>
       <c r="H33" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>156</v>
@@ -2238,7 +2254,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>28</v>
       </c>
@@ -2261,7 +2277,7 @@
         <v>1354</v>
       </c>
       <c r="H34" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>161</v>
@@ -2270,7 +2286,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>12</v>
       </c>
@@ -2302,7 +2318,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>40</v>
       </c>
@@ -2325,7 +2341,7 @@
         <v>108</v>
       </c>
       <c r="H36" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>170</v>
@@ -2334,7 +2350,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>38</v>
       </c>
@@ -2366,7 +2382,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>21</v>
       </c>
@@ -2389,7 +2405,7 @@
         <v>327</v>
       </c>
       <c r="H38" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>179</v>
@@ -2398,7 +2414,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>22</v>
       </c>
@@ -2421,7 +2437,7 @@
         <v>537</v>
       </c>
       <c r="H39" s="2">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>184</v>
@@ -2430,7 +2446,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>49</v>
       </c>
@@ -2453,7 +2469,7 @@
         <v>456</v>
       </c>
       <c r="H40" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>189</v>
@@ -2462,7 +2478,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>19</v>
       </c>
@@ -2494,7 +2510,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2526,7 +2542,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -2558,7 +2574,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>16</v>
       </c>
@@ -2575,7 +2591,7 @@
         <v>13</v>
       </c>
       <c r="F44" s="2">
-        <v>2639</v>
+        <v>2640</v>
       </c>
       <c r="G44" s="2">
         <v>483</v>
@@ -2590,7 +2606,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -2613,7 +2629,7 @@
         <v>381</v>
       </c>
       <c r="H45" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>212</v>
@@ -2622,7 +2638,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>42</v>
       </c>
@@ -2639,7 +2655,7 @@
         <v>13</v>
       </c>
       <c r="F46" s="2">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="G46" s="2">
         <v>131</v>
@@ -2654,7 +2670,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>35</v>
       </c>
@@ -2686,7 +2702,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>18</v>
       </c>
@@ -2718,7 +2734,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>37</v>
       </c>
@@ -2750,7 +2766,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2773,7 +2789,7 @@
         <v>26</v>
       </c>
       <c r="H50" s="2">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>234</v>

</xml_diff>